<commit_message>
Graficos y fotos de graficos
</commit_message>
<xml_diff>
--- a/TP1/Ordenamientos/Graficos.xlsx
+++ b/TP1/Ordenamientos/Graficos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feder\Desktop\tda1\TP1\Ordenamientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DB4D6C-6C43-4B69-97A0-4983ACBECA57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3380DA-F49C-4F34-A260-F98090481734}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,7 +131,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
-    <numFmt numFmtId="173" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -172,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,7 +1138,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2940,7 +2940,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2989,7 +2989,7 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>  arreglo con la invariante 'AntiMerge'</a:t>
+              <a:t>  arreglo con la invariante 'AntiMergeSort'</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4300,8 +4300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="R70" sqref="R70"/>
+    <sheetView tabSelected="1" topLeftCell="G58" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="X70" sqref="X70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5357,12 +5357,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>